<commit_message>
fix color and set f9
</commit_message>
<xml_diff>
--- a/xlsx/model2.xlsx
+++ b/xlsx/model2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\TA_model\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993C34F8-4BB2-44BA-938B-07AF73D96229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53231FB-8365-42FA-A863-CA4EF45305CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21540" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="878" xr2:uid="{BCC5EA96-140E-4D1F-AEAE-F8AA11DA45EB}"/>
   </bookViews>
@@ -43,7 +43,7 @@
   <externalReferences>
     <externalReference r:id="rId27"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1181,9 +1181,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1198,45 +1195,6 @@
     </xf>
     <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1278,18 +1236,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1301,83 +1247,9 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1440,141 +1312,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="6" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1611,16 +1348,335 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="6" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{70DD43AA-AD5B-4D12-80B7-1D771529C2C7}"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="29">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1628,6 +1684,27 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1662,7 +1739,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1670,34 +1747,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -24593,7 +24642,7 @@
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="AH16" sqref="AH16"/>
+      <selection pane="bottomLeft" activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -24615,1184 +24664,1184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="151"/>
-      <c r="B1" s="152"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="100" t="s">
+      <c r="A1" s="85"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="148"/>
-      <c r="H1" s="147" t="s">
+      <c r="F1" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="91"/>
+      <c r="H1" s="90" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="148"/>
+      <c r="I1" s="91"/>
     </row>
     <row r="2" spans="1:31" ht="17.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="154"/>
-      <c r="B2" s="155"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="102" t="s">
+      <c r="A2" s="92"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="95" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="149" t="s">
+      <c r="F2" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="150"/>
-      <c r="H2" s="149" t="s">
+      <c r="G2" s="98"/>
+      <c r="H2" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="150"/>
+      <c r="I2" s="98"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="162" t="s">
+      <c r="A3" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="164" t="s">
+      <c r="B3" s="100" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="165"/>
-      <c r="D3" s="96">
+      <c r="C3" s="101"/>
+      <c r="D3" s="102">
         <v>867</v>
       </c>
-      <c r="E3" s="97">
+      <c r="E3" s="103">
         <v>1067</v>
       </c>
-      <c r="F3" s="157">
+      <c r="F3" s="104">
         <f>1067</f>
         <v>1067</v>
       </c>
-      <c r="G3" s="157"/>
-      <c r="H3" s="160">
+      <c r="G3" s="104"/>
+      <c r="H3" s="105">
         <v>1067</v>
       </c>
-      <c r="I3" s="157"/>
+      <c r="I3" s="104"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="163"/>
-      <c r="B4" s="163" t="s">
+      <c r="A4" s="106"/>
+      <c r="B4" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="166"/>
-      <c r="D4" s="98">
+      <c r="C4" s="107"/>
+      <c r="D4" s="108">
         <v>126</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="109">
         <v>110</v>
       </c>
-      <c r="F4" s="158">
+      <c r="F4" s="110">
         <v>110</v>
       </c>
-      <c r="G4" s="159"/>
-      <c r="H4" s="161">
+      <c r="G4" s="111"/>
+      <c r="H4" s="112">
         <v>110</v>
       </c>
-      <c r="I4" s="159"/>
+      <c r="I4" s="111"/>
       <c r="J4" s="12"/>
-      <c r="Z4" s="117" t="s">
+      <c r="Z4" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="AA4" s="119">
+      <c r="AA4" s="67">
         <v>2010</v>
       </c>
-      <c r="AB4" s="121">
+      <c r="AB4" s="69">
         <v>2020</v>
       </c>
-      <c r="AC4" s="123" t="s">
+      <c r="AC4" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="AD4" s="117" t="s">
+      <c r="AD4" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="AE4" s="115" t="s">
+      <c r="AE4" s="63" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="28" t="s">
+      <c r="C5" s="115"/>
+      <c r="D5" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="92">
+      <c r="E5" s="117">
         <v>1</v>
       </c>
-      <c r="F5" s="136">
+      <c r="F5" s="118">
         <v>1</v>
       </c>
-      <c r="G5" s="137"/>
-      <c r="H5" s="136">
+      <c r="G5" s="119"/>
+      <c r="H5" s="118">
         <v>1</v>
       </c>
-      <c r="I5" s="137"/>
-      <c r="Z5" s="118"/>
-      <c r="AA5" s="120"/>
-      <c r="AB5" s="122"/>
-      <c r="AC5" s="124"/>
-      <c r="AD5" s="118"/>
-      <c r="AE5" s="116"/>
+      <c r="I5" s="119"/>
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="68"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="66"/>
+      <c r="AE5" s="64"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="126"/>
-      <c r="B6" s="61" t="s">
+      <c r="A6" s="120"/>
+      <c r="B6" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="34" t="s">
+      <c r="C6" s="122"/>
+      <c r="D6" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="93">
+      <c r="E6" s="124">
         <v>1</v>
       </c>
-      <c r="F6" s="138">
+      <c r="F6" s="125">
         <v>1</v>
       </c>
-      <c r="G6" s="139"/>
-      <c r="H6" s="138">
+      <c r="G6" s="126"/>
+      <c r="H6" s="125">
         <v>1</v>
       </c>
-      <c r="I6" s="139"/>
-      <c r="Z6" s="64" t="s">
+      <c r="I6" s="126"/>
+      <c r="Z6" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="AA6" s="50">
+      <c r="AA6" s="36">
         <f>CO2排出量!B2</f>
         <v>269.51474216725944</v>
       </c>
-      <c r="AB6" s="56">
+      <c r="AB6" s="42">
         <f>CO2排出量!C2</f>
         <v>209.4235083709562</v>
       </c>
-      <c r="AC6" s="50">
+      <c r="AC6" s="36">
         <v>260.01618074402859</v>
       </c>
-      <c r="AD6" s="56">
+      <c r="AD6" s="42">
         <f>CO2排出量!E2</f>
         <v>260.01618074402859</v>
       </c>
-      <c r="AE6" s="51">
+      <c r="AE6" s="37">
         <f>CO2排出量!F2</f>
         <v>260.01618074402859</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="126"/>
-      <c r="B7" s="62" t="s">
+      <c r="A7" s="120"/>
+      <c r="B7" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="28" t="s">
+      <c r="C7" s="115"/>
+      <c r="D7" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="92">
+      <c r="E7" s="117">
         <v>1</v>
       </c>
-      <c r="F7" s="140">
+      <c r="F7" s="128">
         <v>1</v>
       </c>
-      <c r="G7" s="141"/>
-      <c r="H7" s="140">
+      <c r="G7" s="129"/>
+      <c r="H7" s="128">
         <v>1</v>
       </c>
-      <c r="I7" s="141"/>
-      <c r="Z7" s="99" t="s">
+      <c r="I7" s="129"/>
+      <c r="Z7" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="AA7" s="49">
+      <c r="AA7" s="35">
         <f>CO2排出量!B3</f>
         <v>249.02275586606845</v>
       </c>
-      <c r="AB7" s="57">
+      <c r="AB7" s="43">
         <f>CO2排出量!C3</f>
         <v>196.15609230500672</v>
       </c>
-      <c r="AC7" s="49">
+      <c r="AC7" s="35">
         <v>210.67040851814829</v>
       </c>
-      <c r="AD7" s="57">
+      <c r="AD7" s="43">
         <f>CO2排出量!E3</f>
         <v>210.67040851814829</v>
       </c>
-      <c r="AE7" s="52">
+      <c r="AE7" s="38">
         <f>CO2排出量!F3</f>
         <v>210.67040851814829</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="127"/>
-      <c r="B8" s="63" t="s">
+      <c r="A8" s="130"/>
+      <c r="B8" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="132"/>
+      <c r="D8" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="94">
+      <c r="E8" s="134">
         <v>1</v>
       </c>
-      <c r="F8" s="142">
+      <c r="F8" s="135">
         <v>1</v>
       </c>
-      <c r="G8" s="143"/>
-      <c r="H8" s="142">
+      <c r="G8" s="136"/>
+      <c r="H8" s="135">
         <v>1</v>
       </c>
-      <c r="I8" s="143"/>
-      <c r="Z8" s="65" t="s">
+      <c r="I8" s="136"/>
+      <c r="Z8" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="AA8" s="48">
+      <c r="AA8" s="34">
         <f>CO2排出量!B4</f>
         <v>63.618347666356769</v>
       </c>
-      <c r="AB8" s="58">
+      <c r="AB8" s="44">
         <f>CO2排出量!C4</f>
         <v>52.883709709806709</v>
       </c>
-      <c r="AC8" s="48">
+      <c r="AC8" s="34">
         <v>66.032474177397248</v>
       </c>
-      <c r="AD8" s="58">
+      <c r="AD8" s="44">
         <f>CO2排出量!E4</f>
         <v>66.032474177397248</v>
       </c>
-      <c r="AE8" s="53">
+      <c r="AE8" s="39">
         <f>CO2排出量!F4</f>
         <v>66.032474177397248</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="128" t="s">
+      <c r="A9" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="78">
+      <c r="D9" s="140">
         <v>24</v>
       </c>
-      <c r="E9" s="75">
+      <c r="E9" s="141">
         <v>24</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="142">
         <v>24</v>
       </c>
-      <c r="G9" s="133">
+      <c r="G9" s="143">
         <f>SUM(F9:F13)</f>
         <v>100</v>
       </c>
-      <c r="H9" s="85">
+      <c r="H9" s="144">
         <v>24</v>
       </c>
-      <c r="I9" s="167">
+      <c r="I9" s="145">
         <f>SUM(H9:H13)</f>
         <v>100</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="Z9" s="99" t="s">
+      <c r="Z9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AA9" s="49">
+      <c r="AA9" s="35">
         <f>CO2排出量!B5</f>
         <v>69.588005432578569</v>
       </c>
-      <c r="AB9" s="57">
+      <c r="AB9" s="43">
         <f>CO2排出量!C5</f>
         <v>52.883709709806709</v>
       </c>
-      <c r="AC9" s="49">
+      <c r="AC9" s="35">
         <v>52.527941152998537</v>
       </c>
-      <c r="AD9" s="57">
+      <c r="AD9" s="43">
         <f>CO2排出量!E5</f>
         <v>52.527941152998537</v>
       </c>
-      <c r="AE9" s="52">
+      <c r="AE9" s="38">
         <f>CO2排出量!F5</f>
         <v>52.527941152998537</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="129"/>
-      <c r="B10" s="145"/>
-      <c r="C10" s="40" t="s">
+      <c r="A10" s="146"/>
+      <c r="B10" s="147"/>
+      <c r="C10" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="79">
+      <c r="D10" s="149">
         <v>22</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="150">
         <v>22</v>
       </c>
-      <c r="F10" s="69">
+      <c r="F10" s="151">
         <v>22</v>
       </c>
-      <c r="G10" s="133"/>
-      <c r="H10" s="86">
+      <c r="G10" s="143"/>
+      <c r="H10" s="152">
         <v>22</v>
       </c>
-      <c r="I10" s="168"/>
+      <c r="I10" s="153"/>
       <c r="J10" s="2"/>
-      <c r="Z10" s="65" t="s">
+      <c r="Z10" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="AA10" s="48">
+      <c r="AA10" s="34">
         <f>CO2排出量!B6</f>
         <v>476.37955455993358</v>
       </c>
-      <c r="AB10" s="58">
+      <c r="AB10" s="44">
         <f>CO2排出量!C6</f>
         <v>449.00553720294573</v>
       </c>
-      <c r="AC10" s="48">
+      <c r="AC10" s="34">
         <v>496.52581315955877</v>
       </c>
-      <c r="AD10" s="58">
+      <c r="AD10" s="44">
         <f>CO2排出量!E6</f>
         <v>496.52581315955877</v>
       </c>
-      <c r="AE10" s="53">
+      <c r="AE10" s="39">
         <f>CO2排出量!F6</f>
         <v>496.52581315955877</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="129"/>
-      <c r="B11" s="145"/>
-      <c r="C11" s="41" t="s">
+      <c r="A11" s="146"/>
+      <c r="B11" s="147"/>
+      <c r="C11" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="155">
         <v>14.000000000000002</v>
       </c>
-      <c r="E11" s="72">
+      <c r="E11" s="156">
         <v>14.000000000000002</v>
       </c>
-      <c r="F11" s="68">
+      <c r="F11" s="142">
         <v>14.000000000000002</v>
       </c>
-      <c r="G11" s="133"/>
-      <c r="H11" s="85">
+      <c r="G11" s="143"/>
+      <c r="H11" s="144">
         <v>14.000000000000002</v>
       </c>
-      <c r="I11" s="168"/>
+      <c r="I11" s="153"/>
       <c r="J11" s="2"/>
-      <c r="Z11" s="99" t="s">
+      <c r="Z11" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AA11" s="49">
+      <c r="AA11" s="35">
         <f>CO2排出量!B7</f>
         <v>28.775119328906975</v>
       </c>
-      <c r="AB11" s="57">
+      <c r="AB11" s="43">
         <f>CO2排出量!C7</f>
         <v>25.99212785621209</v>
       </c>
-      <c r="AC11" s="49">
+      <c r="AC11" s="35">
         <v>22.660005374260319</v>
       </c>
-      <c r="AD11" s="57">
+      <c r="AD11" s="43">
         <f>CO2排出量!E7</f>
         <v>22.660005374260319</v>
       </c>
-      <c r="AE11" s="52">
+      <c r="AE11" s="38">
         <f>CO2排出量!F7</f>
         <v>22.660005374260319</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="129"/>
-      <c r="B12" s="145"/>
-      <c r="C12" s="40" t="s">
+      <c r="A12" s="146"/>
+      <c r="B12" s="147"/>
+      <c r="C12" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="79">
+      <c r="D12" s="149">
         <v>4</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="150">
         <v>4</v>
       </c>
-      <c r="F12" s="69">
+      <c r="F12" s="151">
         <v>4</v>
       </c>
-      <c r="G12" s="133"/>
-      <c r="H12" s="86">
+      <c r="G12" s="143"/>
+      <c r="H12" s="152">
         <v>4</v>
       </c>
-      <c r="I12" s="168"/>
+      <c r="I12" s="153"/>
       <c r="J12" s="2"/>
-      <c r="Z12" s="65" t="s">
+      <c r="Z12" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="AA12" s="48">
+      <c r="AA12" s="34">
         <f>CO2排出量!B8</f>
         <v>29.46362437612942</v>
       </c>
-      <c r="AB12" s="58">
+      <c r="AB12" s="44">
         <f>CO2排出量!C8</f>
         <v>31.085649151718691</v>
       </c>
-      <c r="AC12" s="48">
+      <c r="AC12" s="34">
         <v>27.100550625829783</v>
       </c>
-      <c r="AD12" s="58">
+      <c r="AD12" s="44">
         <f>CO2排出量!E8</f>
         <v>27.100550625829783</v>
       </c>
-      <c r="AE12" s="53">
+      <c r="AE12" s="39">
         <f>CO2排出量!F8</f>
         <v>27.100550625829783</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="129"/>
-      <c r="B13" s="146"/>
-      <c r="C13" s="42" t="s">
+      <c r="A13" s="146"/>
+      <c r="B13" s="157"/>
+      <c r="C13" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="81">
+      <c r="D13" s="159">
         <v>36</v>
       </c>
-      <c r="E13" s="76">
+      <c r="E13" s="160">
         <v>36</v>
       </c>
-      <c r="F13" s="70">
+      <c r="F13" s="161">
         <v>36</v>
       </c>
-      <c r="G13" s="134"/>
-      <c r="H13" s="87">
+      <c r="G13" s="162"/>
+      <c r="H13" s="163">
         <v>36</v>
       </c>
-      <c r="I13" s="169"/>
+      <c r="I13" s="164"/>
       <c r="J13" s="2"/>
-      <c r="Z13" s="99" t="s">
+      <c r="Z13" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="AA13" s="49">
+      <c r="AA13" s="35">
         <f>CO2排出量!B9</f>
         <v>-46</v>
       </c>
-      <c r="AB13" s="57">
+      <c r="AB13" s="43">
         <f>CO2排出量!C9</f>
         <v>-46</v>
       </c>
-      <c r="AC13" s="49">
+      <c r="AC13" s="35">
         <v>-46</v>
       </c>
-      <c r="AD13" s="57">
+      <c r="AD13" s="43">
         <f>CO2排出量!E9</f>
         <v>-46</v>
       </c>
-      <c r="AE13" s="52">
+      <c r="AE13" s="38">
         <f>CO2排出量!F9</f>
         <v>-46</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="129"/>
-      <c r="B14" s="144" t="s">
+      <c r="A14" s="146"/>
+      <c r="B14" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="82">
-        <v>0</v>
-      </c>
-      <c r="E14" s="71">
-        <v>0</v>
-      </c>
-      <c r="F14" s="71">
-        <v>0</v>
-      </c>
-      <c r="G14" s="135">
+      <c r="D14" s="166">
+        <v>0</v>
+      </c>
+      <c r="E14" s="167">
+        <v>0</v>
+      </c>
+      <c r="F14" s="167">
+        <v>0</v>
+      </c>
+      <c r="G14" s="168">
         <f t="shared" ref="G14" si="0">SUM(F14:F18)</f>
         <v>100</v>
       </c>
-      <c r="H14" s="88">
-        <v>0</v>
-      </c>
-      <c r="I14" s="167">
+      <c r="H14" s="169">
+        <v>0</v>
+      </c>
+      <c r="I14" s="145">
         <f>SUM(H14:H18)</f>
         <v>100</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="Z14" s="66" t="s">
+      <c r="Z14" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="AA14" s="54">
+      <c r="AA14" s="40">
         <f>CO2排出量!B10</f>
         <v>1140.3621493972332</v>
       </c>
-      <c r="AB14" s="59">
+      <c r="AB14" s="45">
         <f>CO2排出量!C10</f>
         <v>971.43033430645278</v>
       </c>
-      <c r="AC14" s="54">
+      <c r="AC14" s="40">
         <v>1089.5333737522215</v>
       </c>
-      <c r="AD14" s="59">
+      <c r="AD14" s="45">
         <f>CO2排出量!E10</f>
         <v>1089.5333737522215</v>
       </c>
-      <c r="AE14" s="55">
+      <c r="AE14" s="41">
         <f>CO2排出量!F10</f>
         <v>1089.5333737522215</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="129"/>
-      <c r="B15" s="145"/>
-      <c r="C15" s="41" t="s">
+      <c r="A15" s="146"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="155">
         <v>97</v>
       </c>
-      <c r="E15" s="72">
+      <c r="E15" s="156">
         <v>97</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="156">
         <v>97</v>
       </c>
-      <c r="G15" s="133"/>
-      <c r="H15" s="85">
+      <c r="G15" s="143"/>
+      <c r="H15" s="144">
         <v>97</v>
       </c>
-      <c r="I15" s="168"/>
+      <c r="I15" s="153"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="129"/>
-      <c r="B16" s="145"/>
-      <c r="C16" s="40" t="s">
+      <c r="A16" s="146"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="79">
-        <v>0</v>
-      </c>
-      <c r="E16" s="73">
-        <v>0</v>
-      </c>
-      <c r="F16" s="73">
-        <v>0</v>
-      </c>
-      <c r="G16" s="133"/>
-      <c r="H16" s="86">
-        <v>0</v>
-      </c>
-      <c r="I16" s="168"/>
+      <c r="D16" s="149">
+        <v>0</v>
+      </c>
+      <c r="E16" s="150">
+        <v>0</v>
+      </c>
+      <c r="F16" s="150">
+        <v>0</v>
+      </c>
+      <c r="G16" s="143"/>
+      <c r="H16" s="152">
+        <v>0</v>
+      </c>
+      <c r="I16" s="153"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="129"/>
-      <c r="B17" s="145"/>
-      <c r="C17" s="41" t="s">
+      <c r="A17" s="146"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="80">
+      <c r="D17" s="155">
         <v>1</v>
       </c>
-      <c r="E17" s="72">
+      <c r="E17" s="156">
         <v>1</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17" s="156">
         <v>1</v>
       </c>
-      <c r="G17" s="133"/>
-      <c r="H17" s="85">
+      <c r="G17" s="143"/>
+      <c r="H17" s="144">
         <v>1</v>
       </c>
-      <c r="I17" s="168"/>
+      <c r="I17" s="153"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="129"/>
-      <c r="B18" s="146"/>
-      <c r="C18" s="44" t="s">
+      <c r="A18" s="146"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="170" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="83">
+      <c r="D18" s="171">
         <v>2</v>
       </c>
-      <c r="E18" s="74">
+      <c r="E18" s="172">
         <v>2</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="172">
         <v>2</v>
       </c>
-      <c r="G18" s="134"/>
-      <c r="H18" s="89">
+      <c r="G18" s="162"/>
+      <c r="H18" s="173">
         <v>2</v>
       </c>
-      <c r="I18" s="169"/>
+      <c r="I18" s="164"/>
       <c r="J18" s="2"/>
-      <c r="AE18" s="104"/>
+      <c r="AE18" s="52"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="129"/>
-      <c r="B19" s="144" t="s">
+      <c r="A19" s="146"/>
+      <c r="B19" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="78">
-        <v>0</v>
-      </c>
-      <c r="E19" s="75">
-        <v>0</v>
-      </c>
-      <c r="F19" s="75">
-        <v>0</v>
-      </c>
-      <c r="G19" s="135">
+      <c r="D19" s="140">
+        <v>0</v>
+      </c>
+      <c r="E19" s="141">
+        <v>0</v>
+      </c>
+      <c r="F19" s="141">
+        <v>0</v>
+      </c>
+      <c r="G19" s="168">
         <f t="shared" ref="G19" si="1">SUM(F19:F23)</f>
         <v>100</v>
       </c>
-      <c r="H19" s="90">
-        <v>0</v>
-      </c>
-      <c r="I19" s="167">
+      <c r="H19" s="174">
+        <v>0</v>
+      </c>
+      <c r="I19" s="145">
         <f>SUM(H19:H23)</f>
         <v>100</v>
       </c>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="129"/>
-      <c r="B20" s="145"/>
-      <c r="C20" s="40" t="s">
+      <c r="A20" s="146"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="79">
+      <c r="D20" s="149">
         <v>24</v>
       </c>
-      <c r="E20" s="73">
+      <c r="E20" s="150">
         <v>24</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="150">
         <v>24</v>
       </c>
-      <c r="G20" s="133"/>
-      <c r="H20" s="86">
+      <c r="G20" s="143"/>
+      <c r="H20" s="152">
         <v>24</v>
       </c>
-      <c r="I20" s="168"/>
+      <c r="I20" s="153"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="129"/>
-      <c r="B21" s="145"/>
-      <c r="C21" s="41" t="s">
+      <c r="A21" s="146"/>
+      <c r="B21" s="147"/>
+      <c r="C21" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="80">
+      <c r="D21" s="155">
         <v>16</v>
       </c>
-      <c r="E21" s="72">
+      <c r="E21" s="156">
         <v>16</v>
       </c>
-      <c r="F21" s="72">
+      <c r="F21" s="156">
         <v>16</v>
       </c>
-      <c r="G21" s="133"/>
-      <c r="H21" s="85">
+      <c r="G21" s="143"/>
+      <c r="H21" s="144">
         <v>16</v>
       </c>
-      <c r="I21" s="168"/>
+      <c r="I21" s="153"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="129"/>
-      <c r="B22" s="145"/>
-      <c r="C22" s="40" t="s">
+      <c r="A22" s="146"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="79">
+      <c r="D22" s="149">
         <v>3</v>
       </c>
-      <c r="E22" s="73">
+      <c r="E22" s="150">
         <v>3</v>
       </c>
-      <c r="F22" s="73">
+      <c r="F22" s="150">
         <v>3</v>
       </c>
-      <c r="G22" s="133"/>
-      <c r="H22" s="86">
+      <c r="G22" s="143"/>
+      <c r="H22" s="152">
         <v>3</v>
       </c>
-      <c r="I22" s="168"/>
+      <c r="I22" s="153"/>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="129"/>
-      <c r="B23" s="146"/>
-      <c r="C23" s="42" t="s">
+      <c r="A23" s="146"/>
+      <c r="B23" s="157"/>
+      <c r="C23" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="81">
+      <c r="D23" s="159">
         <v>56.999999999999993</v>
       </c>
-      <c r="E23" s="76">
+      <c r="E23" s="160">
         <v>56.999999999999993</v>
       </c>
-      <c r="F23" s="76">
+      <c r="F23" s="160">
         <v>56.999999999999993</v>
       </c>
-      <c r="G23" s="134"/>
-      <c r="H23" s="87">
+      <c r="G23" s="162"/>
+      <c r="H23" s="163">
         <v>56.999999999999993</v>
       </c>
-      <c r="I23" s="169"/>
+      <c r="I23" s="164"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="129"/>
-      <c r="B24" s="144" t="s">
+      <c r="A24" s="146"/>
+      <c r="B24" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="82">
-        <v>0</v>
-      </c>
-      <c r="E24" s="71">
-        <v>0</v>
-      </c>
-      <c r="F24" s="71">
-        <v>0</v>
-      </c>
-      <c r="G24" s="135">
+      <c r="D24" s="166">
+        <v>0</v>
+      </c>
+      <c r="E24" s="167">
+        <v>0</v>
+      </c>
+      <c r="F24" s="167">
+        <v>0</v>
+      </c>
+      <c r="G24" s="168">
         <f t="shared" ref="G24" si="2">SUM(F24:F28)</f>
         <v>100</v>
       </c>
-      <c r="H24" s="88">
-        <v>0</v>
-      </c>
-      <c r="I24" s="167">
+      <c r="H24" s="169">
+        <v>0</v>
+      </c>
+      <c r="I24" s="145">
         <f>SUM(H24:H28)</f>
         <v>100</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="129"/>
-      <c r="B25" s="145"/>
-      <c r="C25" s="41" t="s">
+      <c r="A25" s="146"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="80">
+      <c r="D25" s="155">
         <v>27</v>
       </c>
-      <c r="E25" s="72">
+      <c r="E25" s="156">
         <v>27</v>
       </c>
-      <c r="F25" s="72">
+      <c r="F25" s="156">
         <v>27</v>
       </c>
-      <c r="G25" s="133"/>
-      <c r="H25" s="85">
+      <c r="G25" s="143"/>
+      <c r="H25" s="144">
         <v>27</v>
       </c>
-      <c r="I25" s="168"/>
+      <c r="I25" s="153"/>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="129"/>
-      <c r="B26" s="145"/>
-      <c r="C26" s="40" t="s">
+      <c r="A26" s="146"/>
+      <c r="B26" s="147"/>
+      <c r="C26" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="79">
+      <c r="D26" s="149">
         <v>21</v>
       </c>
-      <c r="E26" s="73">
+      <c r="E26" s="150">
         <v>21</v>
       </c>
-      <c r="F26" s="73">
+      <c r="F26" s="150">
         <v>21</v>
       </c>
-      <c r="G26" s="133"/>
-      <c r="H26" s="86">
+      <c r="G26" s="143"/>
+      <c r="H26" s="152">
         <v>21</v>
       </c>
-      <c r="I26" s="168"/>
+      <c r="I26" s="153"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="129"/>
-      <c r="B27" s="145"/>
-      <c r="C27" s="41" t="s">
+      <c r="A27" s="146"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="80">
-        <v>0</v>
-      </c>
-      <c r="E27" s="72">
-        <v>0</v>
-      </c>
-      <c r="F27" s="72">
-        <v>0</v>
-      </c>
-      <c r="G27" s="133"/>
-      <c r="H27" s="85">
-        <v>0</v>
-      </c>
-      <c r="I27" s="168"/>
+      <c r="D27" s="155">
+        <v>0</v>
+      </c>
+      <c r="E27" s="156">
+        <v>0</v>
+      </c>
+      <c r="F27" s="156">
+        <v>0</v>
+      </c>
+      <c r="G27" s="143"/>
+      <c r="H27" s="144">
+        <v>0</v>
+      </c>
+      <c r="I27" s="153"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="129"/>
-      <c r="B28" s="146"/>
-      <c r="C28" s="44" t="s">
+      <c r="A28" s="146"/>
+      <c r="B28" s="157"/>
+      <c r="C28" s="170" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="83">
+      <c r="D28" s="171">
         <v>52</v>
       </c>
-      <c r="E28" s="74">
+      <c r="E28" s="172">
         <v>52</v>
       </c>
-      <c r="F28" s="74">
+      <c r="F28" s="172">
         <v>52</v>
       </c>
-      <c r="G28" s="134"/>
-      <c r="H28" s="89">
+      <c r="G28" s="162"/>
+      <c r="H28" s="173">
         <v>52</v>
       </c>
-      <c r="I28" s="169"/>
+      <c r="I28" s="164"/>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="130" t="s">
+      <c r="A29" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="144" t="s">
+      <c r="B29" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="78">
+      <c r="D29" s="140">
         <v>31</v>
       </c>
-      <c r="E29" s="75">
+      <c r="E29" s="141">
         <v>31</v>
       </c>
-      <c r="F29" s="75">
+      <c r="F29" s="141">
         <v>31</v>
       </c>
-      <c r="G29" s="135">
+      <c r="G29" s="168">
         <f>SUM(F29:F41)</f>
         <v>100</v>
       </c>
-      <c r="H29" s="90">
+      <c r="H29" s="174">
         <v>31</v>
       </c>
-      <c r="I29" s="167">
+      <c r="I29" s="145">
         <f>SUM(H29:H41)</f>
         <v>100</v>
       </c>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="131"/>
-      <c r="B30" s="145"/>
-      <c r="C30" s="45" t="s">
+      <c r="A30" s="176"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="177" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="84">
-        <v>0</v>
-      </c>
-      <c r="E30" s="77">
-        <v>0</v>
-      </c>
-      <c r="F30" s="77">
-        <v>0</v>
-      </c>
-      <c r="G30" s="133"/>
-      <c r="H30" s="91">
-        <v>0</v>
-      </c>
-      <c r="I30" s="168"/>
+      <c r="D30" s="178">
+        <v>0</v>
+      </c>
+      <c r="E30" s="179">
+        <v>0</v>
+      </c>
+      <c r="F30" s="179">
+        <v>0</v>
+      </c>
+      <c r="G30" s="143"/>
+      <c r="H30" s="180">
+        <v>0</v>
+      </c>
+      <c r="I30" s="153"/>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="131"/>
-      <c r="B31" s="145"/>
-      <c r="C31" s="41" t="s">
+      <c r="A31" s="176"/>
+      <c r="B31" s="147"/>
+      <c r="C31" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="80">
+      <c r="D31" s="155">
         <v>3</v>
       </c>
-      <c r="E31" s="72">
+      <c r="E31" s="156">
         <v>3</v>
       </c>
-      <c r="F31" s="72">
+      <c r="F31" s="156">
         <v>3</v>
       </c>
-      <c r="G31" s="133"/>
-      <c r="H31" s="85">
+      <c r="G31" s="143"/>
+      <c r="H31" s="144">
         <v>3</v>
       </c>
-      <c r="I31" s="168"/>
+      <c r="I31" s="153"/>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="131"/>
-      <c r="B32" s="145"/>
-      <c r="C32" s="45" t="s">
+      <c r="A32" s="176"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="177" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="84">
-        <v>0</v>
-      </c>
-      <c r="E32" s="77">
-        <v>0</v>
-      </c>
-      <c r="F32" s="77">
-        <v>0</v>
-      </c>
-      <c r="G32" s="133"/>
-      <c r="H32" s="91">
-        <v>0</v>
-      </c>
-      <c r="I32" s="168"/>
+      <c r="D32" s="178">
+        <v>0</v>
+      </c>
+      <c r="E32" s="179">
+        <v>0</v>
+      </c>
+      <c r="F32" s="179">
+        <v>0</v>
+      </c>
+      <c r="G32" s="143"/>
+      <c r="H32" s="180">
+        <v>0</v>
+      </c>
+      <c r="I32" s="153"/>
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="131"/>
-      <c r="B33" s="145"/>
-      <c r="C33" s="41" t="s">
+      <c r="A33" s="176"/>
+      <c r="B33" s="147"/>
+      <c r="C33" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="80">
+      <c r="D33" s="155">
         <v>40</v>
       </c>
-      <c r="E33" s="72">
+      <c r="E33" s="156">
         <v>40</v>
       </c>
-      <c r="F33" s="72">
+      <c r="F33" s="156">
         <v>40</v>
       </c>
-      <c r="G33" s="133"/>
-      <c r="H33" s="85">
+      <c r="G33" s="143"/>
+      <c r="H33" s="144">
         <v>40</v>
       </c>
-      <c r="I33" s="168"/>
+      <c r="I33" s="153"/>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="131"/>
-      <c r="B34" s="145"/>
-      <c r="C34" s="45" t="s">
+      <c r="A34" s="176"/>
+      <c r="B34" s="147"/>
+      <c r="C34" s="177" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="84">
-        <v>0</v>
-      </c>
-      <c r="E34" s="77">
-        <v>0</v>
-      </c>
-      <c r="F34" s="77">
-        <v>0</v>
-      </c>
-      <c r="G34" s="133"/>
-      <c r="H34" s="91">
-        <v>0</v>
-      </c>
-      <c r="I34" s="168"/>
+      <c r="D34" s="178">
+        <v>0</v>
+      </c>
+      <c r="E34" s="179">
+        <v>0</v>
+      </c>
+      <c r="F34" s="179">
+        <v>0</v>
+      </c>
+      <c r="G34" s="143"/>
+      <c r="H34" s="180">
+        <v>0</v>
+      </c>
+      <c r="I34" s="153"/>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="131"/>
-      <c r="B35" s="145"/>
-      <c r="C35" s="41" t="s">
+      <c r="A35" s="176"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="154" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="80">
+      <c r="D35" s="155">
         <v>4</v>
       </c>
-      <c r="E35" s="72">
+      <c r="E35" s="156">
         <v>4</v>
       </c>
-      <c r="F35" s="72">
+      <c r="F35" s="156">
         <v>4</v>
       </c>
-      <c r="G35" s="133"/>
-      <c r="H35" s="85">
+      <c r="G35" s="143"/>
+      <c r="H35" s="144">
         <v>4</v>
       </c>
-      <c r="I35" s="168"/>
+      <c r="I35" s="153"/>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="131"/>
-      <c r="B36" s="145"/>
-      <c r="C36" s="45" t="s">
+      <c r="A36" s="176"/>
+      <c r="B36" s="147"/>
+      <c r="C36" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="84">
+      <c r="D36" s="178">
         <v>5</v>
       </c>
-      <c r="E36" s="77">
+      <c r="E36" s="179">
         <v>5</v>
       </c>
-      <c r="F36" s="77">
+      <c r="F36" s="179">
         <v>5</v>
       </c>
-      <c r="G36" s="133"/>
-      <c r="H36" s="91">
+      <c r="G36" s="143"/>
+      <c r="H36" s="180">
         <v>5</v>
       </c>
-      <c r="I36" s="168"/>
+      <c r="I36" s="153"/>
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="131"/>
-      <c r="B37" s="145"/>
-      <c r="C37" s="41" t="s">
+      <c r="A37" s="176"/>
+      <c r="B37" s="147"/>
+      <c r="C37" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="80">
-        <v>0</v>
-      </c>
-      <c r="E37" s="72">
-        <v>0</v>
-      </c>
-      <c r="F37" s="72">
-        <v>0</v>
-      </c>
-      <c r="G37" s="133"/>
-      <c r="H37" s="85">
-        <v>0</v>
-      </c>
-      <c r="I37" s="168"/>
+      <c r="D37" s="155">
+        <v>0</v>
+      </c>
+      <c r="E37" s="156">
+        <v>0</v>
+      </c>
+      <c r="F37" s="156">
+        <v>0</v>
+      </c>
+      <c r="G37" s="143"/>
+      <c r="H37" s="144">
+        <v>0</v>
+      </c>
+      <c r="I37" s="153"/>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="131"/>
-      <c r="B38" s="145"/>
-      <c r="C38" s="45" t="s">
+      <c r="A38" s="176"/>
+      <c r="B38" s="147"/>
+      <c r="C38" s="177" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="84">
+      <c r="D38" s="178">
         <v>8</v>
       </c>
-      <c r="E38" s="77">
+      <c r="E38" s="179">
         <v>8</v>
       </c>
-      <c r="F38" s="77">
+      <c r="F38" s="179">
         <v>8</v>
       </c>
-      <c r="G38" s="133"/>
-      <c r="H38" s="91">
+      <c r="G38" s="143"/>
+      <c r="H38" s="180">
         <v>8</v>
       </c>
-      <c r="I38" s="168"/>
+      <c r="I38" s="153"/>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="131"/>
-      <c r="B39" s="145"/>
-      <c r="C39" s="41" t="s">
+      <c r="A39" s="176"/>
+      <c r="B39" s="147"/>
+      <c r="C39" s="154" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="80">
-        <v>0</v>
-      </c>
-      <c r="E39" s="72">
-        <v>0</v>
-      </c>
-      <c r="F39" s="72">
-        <v>0</v>
-      </c>
-      <c r="G39" s="133"/>
-      <c r="H39" s="85">
-        <v>0</v>
-      </c>
-      <c r="I39" s="168"/>
+      <c r="D39" s="155">
+        <v>0</v>
+      </c>
+      <c r="E39" s="156">
+        <v>0</v>
+      </c>
+      <c r="F39" s="156">
+        <v>0</v>
+      </c>
+      <c r="G39" s="143"/>
+      <c r="H39" s="144">
+        <v>0</v>
+      </c>
+      <c r="I39" s="153"/>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="131"/>
-      <c r="B40" s="145"/>
-      <c r="C40" s="45" t="s">
+      <c r="A40" s="176"/>
+      <c r="B40" s="147"/>
+      <c r="C40" s="177" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="84">
+      <c r="D40" s="178">
         <v>1</v>
       </c>
-      <c r="E40" s="77">
+      <c r="E40" s="179">
         <v>1</v>
       </c>
-      <c r="F40" s="77">
+      <c r="F40" s="179">
         <v>1</v>
       </c>
-      <c r="G40" s="133"/>
-      <c r="H40" s="91">
+      <c r="G40" s="143"/>
+      <c r="H40" s="180">
         <v>1</v>
       </c>
-      <c r="I40" s="168"/>
+      <c r="I40" s="153"/>
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="132"/>
-      <c r="B41" s="146"/>
-      <c r="C41" s="42" t="s">
+      <c r="A41" s="181"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="158" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="81">
+      <c r="D41" s="159">
         <v>8</v>
       </c>
-      <c r="E41" s="76">
+      <c r="E41" s="160">
         <v>8</v>
       </c>
-      <c r="F41" s="76">
+      <c r="F41" s="160">
         <v>8</v>
       </c>
-      <c r="G41" s="134"/>
-      <c r="H41" s="87">
+      <c r="G41" s="162"/>
+      <c r="H41" s="163">
         <v>8</v>
       </c>
-      <c r="I41" s="169"/>
+      <c r="I41" s="164"/>
       <c r="J41" s="2"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="113"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
+      <c r="A43" s="61"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="114"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67"/>
+      <c r="A44" s="62"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D45" s="67"/>
+      <c r="D45" s="49"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D46" s="67"/>
+      <c r="D46" s="49"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="17"/>
@@ -25838,28 +25887,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B29:B41"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="I9:I13"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="I19:I23"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="I29:I41"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="AE4:AE5"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AB4:AB5"/>
+    <mergeCell ref="AC4:AC5"/>
+    <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A28"/>
     <mergeCell ref="A29:A41"/>
@@ -25876,121 +25909,158 @@
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="B24:B28"/>
-    <mergeCell ref="AE4:AE5"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AA4:AA5"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="AC4:AC5"/>
-    <mergeCell ref="AD4:AD5"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B29:B41"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="I19:I23"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="I29:I41"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="G14">
-    <cfRule type="expression" dxfId="21" priority="23">
+    <cfRule type="expression" dxfId="28" priority="31">
       <formula>$G$14&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="27" priority="27">
       <formula>$G$9&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>$I$19&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="25" priority="29">
       <formula>$G$29&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>$G$24&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>$I$9&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="22" priority="24">
       <formula>$I$14&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>$G$19&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>$I$24&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>$I$29&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:F28">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="5" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H28">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="7" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:I8">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="3" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:F41">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H41">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="18" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:I4">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="1" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z6:AE14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z4:AE5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31105,20 +31175,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="179" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -32951,27 +33021,27 @@
         <f>シナリオ!F11/100</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="E46" s="95">
+      <c r="E46" s="50">
         <f>シナリオ!F12/100</f>
         <v>0.04</v>
       </c>
-      <c r="F46" s="95">
+      <c r="F46" s="50">
         <f>シナリオ!F13/100</f>
         <v>0.36</v>
       </c>
-      <c r="G46" s="95">
+      <c r="G46" s="50">
         <f>シナリオ!H9/100</f>
         <v>0.24</v>
       </c>
-      <c r="H46" s="95">
+      <c r="H46" s="50">
         <f>シナリオ!H10/100</f>
         <v>0.22</v>
       </c>
-      <c r="I46" s="95">
+      <c r="I46" s="50">
         <f>シナリオ!H11/100</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="J46" s="95">
+      <c r="J46" s="50">
         <f>シナリオ!H12/100</f>
         <v>0.04</v>
       </c>
@@ -33007,20 +33077,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="179" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -34907,20 +34977,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="179" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -36807,20 +36877,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="179" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -38707,36 +38777,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="180" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="181"/>
-      <c r="O1" s="180" t="s">
+      <c r="B1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -43137,7 +43207,7 @@
         <f>シナリオ!F33/100</f>
         <v>0.4</v>
       </c>
-      <c r="G46" s="95">
+      <c r="G46" s="50">
         <f>シナリオ!F34/100</f>
         <v>0</v>
       </c>
@@ -43149,7 +43219,7 @@
         <f>シナリオ!F36/100</f>
         <v>0.05</v>
       </c>
-      <c r="J46" s="95">
+      <c r="J46" s="50">
         <f>シナリオ!F37/100</f>
         <v>0</v>
       </c>
@@ -43254,61 +43324,61 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="170" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="173" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="174"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="77"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="111" t="s">
+      <c r="F2" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="112" t="s">
+      <c r="G2" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="111" t="s">
+      <c r="H2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="111" t="s">
+      <c r="I2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="111" t="s">
+      <c r="J2" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="111" t="s">
+      <c r="K2" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="112" t="s">
+      <c r="L2" s="60" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="109">
+      <c r="B3" s="57">
         <v>2010</v>
       </c>
       <c r="C3" s="10">
@@ -43327,7 +43397,7 @@
         <f>'Consumption(EJyr)'!$B$2*sIND!E3</f>
         <v>0.13971205722135449</v>
       </c>
-      <c r="G3" s="105">
+      <c r="G3" s="53">
         <f>'Consumption(EJyr)'!$B$2*sIND!F3</f>
         <v>1.3636103186366102</v>
       </c>
@@ -43347,14 +43417,14 @@
         <f>'Consumption(EJyr)'!$C$2*sIND!J3</f>
         <v>0.13971205722135449</v>
       </c>
-      <c r="L3" s="105">
+      <c r="L3" s="53">
         <f>'Consumption(EJyr)'!$C$2*sIND!K3</f>
         <v>1.3636103186366102</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="107"/>
-      <c r="B4" s="107">
+      <c r="A4" s="55"/>
+      <c r="B4" s="55">
         <v>2020</v>
       </c>
       <c r="C4" s="9">
@@ -43399,8 +43469,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="107"/>
-      <c r="B5" s="107">
+      <c r="A5" s="55"/>
+      <c r="B5" s="55">
         <v>2030</v>
       </c>
       <c r="C5" s="9">
@@ -43445,8 +43515,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="107"/>
-      <c r="B6" s="107">
+      <c r="A6" s="55"/>
+      <c r="B6" s="55">
         <v>2040</v>
       </c>
       <c r="C6" s="9">
@@ -43491,8 +43561,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="108"/>
-      <c r="B7" s="108">
+      <c r="A7" s="56"/>
+      <c r="B7" s="56">
         <v>2050</v>
       </c>
       <c r="C7" s="8">
@@ -43537,10 +43607,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="107">
+      <c r="B8" s="55">
         <v>2010</v>
       </c>
       <c r="C8" s="9">
@@ -43585,8 +43655,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="107"/>
-      <c r="B9" s="107">
+      <c r="A9" s="55"/>
+      <c r="B9" s="55">
         <v>2020</v>
       </c>
       <c r="C9" s="9">
@@ -43631,8 +43701,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="107"/>
-      <c r="B10" s="107">
+      <c r="A10" s="55"/>
+      <c r="B10" s="55">
         <v>2030</v>
       </c>
       <c r="C10" s="9">
@@ -43677,8 +43747,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="107"/>
-      <c r="B11" s="107">
+      <c r="A11" s="55"/>
+      <c r="B11" s="55">
         <v>2040</v>
       </c>
       <c r="C11" s="9">
@@ -43723,8 +43793,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="107"/>
-      <c r="B12" s="107">
+      <c r="A12" s="55"/>
+      <c r="B12" s="55">
         <v>2050</v>
       </c>
       <c r="C12" s="9">
@@ -43769,10 +43839,10 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="109">
+      <c r="B13" s="57">
         <v>2010</v>
       </c>
       <c r="C13" s="10">
@@ -43791,7 +43861,7 @@
         <f>'Consumption(EJyr)'!$F$2*sCOM!E3</f>
         <v>5.5761227810565077E-2</v>
       </c>
-      <c r="G13" s="105">
+      <c r="G13" s="53">
         <f>'Consumption(EJyr)'!$F$2*sCOM!F3</f>
         <v>1.2272144966755287</v>
       </c>
@@ -43811,14 +43881,14 @@
         <f>'Consumption(EJyr)'!$G$2*sCOM!J3</f>
         <v>5.5761227810565077E-2</v>
       </c>
-      <c r="L13" s="105">
+      <c r="L13" s="53">
         <f>'Consumption(EJyr)'!$G$2*sCOM!K3</f>
         <v>1.2272144966755287</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="107"/>
-      <c r="B14" s="107">
+      <c r="A14" s="55"/>
+      <c r="B14" s="55">
         <v>2020</v>
       </c>
       <c r="C14" s="9">
@@ -43863,8 +43933,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="107"/>
-      <c r="B15" s="107">
+      <c r="A15" s="55"/>
+      <c r="B15" s="55">
         <v>2030</v>
       </c>
       <c r="C15" s="9">
@@ -43909,8 +43979,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="107"/>
-      <c r="B16" s="107">
+      <c r="A16" s="55"/>
+      <c r="B16" s="55">
         <v>2040</v>
       </c>
       <c r="C16" s="9">
@@ -43955,8 +44025,8 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="108"/>
-      <c r="B17" s="108">
+      <c r="A17" s="56"/>
+      <c r="B17" s="56">
         <v>2050</v>
       </c>
       <c r="C17" s="8">
@@ -44001,10 +44071,10 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="107" t="s">
+      <c r="A18" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="107">
+      <c r="B18" s="55">
         <v>2010</v>
       </c>
       <c r="C18" s="9">
@@ -44049,8 +44119,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="107"/>
-      <c r="B19" s="107">
+      <c r="A19" s="55"/>
+      <c r="B19" s="55">
         <v>2020</v>
       </c>
       <c r="C19" s="9">
@@ -44095,8 +44165,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="107"/>
-      <c r="B20" s="107">
+      <c r="A20" s="55"/>
+      <c r="B20" s="55">
         <v>2030</v>
       </c>
       <c r="C20" s="9">
@@ -44141,8 +44211,8 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="107"/>
-      <c r="B21" s="107">
+      <c r="A21" s="55"/>
+      <c r="B21" s="55">
         <v>2040</v>
       </c>
       <c r="C21" s="9">
@@ -44187,8 +44257,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="107"/>
-      <c r="B22" s="107">
+      <c r="A22" s="55"/>
+      <c r="B22" s="55">
         <v>2050</v>
       </c>
       <c r="C22" s="9">
@@ -44233,10 +44303,10 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="109" t="s">
+      <c r="A23" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="109">
+      <c r="B23" s="57">
         <v>2010</v>
       </c>
       <c r="C23" s="10">
@@ -44255,7 +44325,7 @@
         <f t="shared" si="0"/>
         <v>0.20418016053948937</v>
       </c>
-      <c r="G23" s="105">
+      <c r="G23" s="53">
         <f t="shared" si="0"/>
         <v>3.7404319113217492</v>
       </c>
@@ -44275,14 +44345,14 @@
         <f t="shared" si="0"/>
         <v>0.20418016053948937</v>
       </c>
-      <c r="L23" s="105">
+      <c r="L23" s="53">
         <f t="shared" si="0"/>
         <v>3.7404319113217492</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="107"/>
-      <c r="B24" s="107">
+      <c r="A24" s="55"/>
+      <c r="B24" s="55">
         <v>2020</v>
       </c>
       <c r="C24" s="9">
@@ -44327,8 +44397,8 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="107"/>
-      <c r="B25" s="107">
+      <c r="A25" s="55"/>
+      <c r="B25" s="55">
         <v>2030</v>
       </c>
       <c r="C25" s="9">
@@ -44373,8 +44443,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="107"/>
-      <c r="B26" s="107">
+      <c r="A26" s="55"/>
+      <c r="B26" s="55">
         <v>2040</v>
       </c>
       <c r="C26" s="9">
@@ -44419,8 +44489,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="108"/>
-      <c r="B27" s="108">
+      <c r="A27" s="56"/>
+      <c r="B27" s="56">
         <v>2050</v>
       </c>
       <c r="C27" s="8">
@@ -46536,14 +46606,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="180" t="s">
+      <c r="B1" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="180"/>
+      <c r="E1" s="83"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -47284,14 +47354,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="180" t="s">
+      <c r="B1" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="180"/>
+      <c r="E1" s="83"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -48325,10 +48395,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D1" s="180" t="s">
+      <c r="D1" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="180"/>
+      <c r="E1" s="83"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
@@ -49249,41 +49319,41 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10"/>
-      <c r="B1" s="173" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="174"/>
-      <c r="P1" s="173" t="s">
+      <c r="B1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="174"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="77"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="54" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -49325,7 +49395,7 @@
       <c r="N2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="105" t="s">
+      <c r="O2" s="53" t="s">
         <v>27</v>
       </c>
       <c r="P2" s="10" t="s">
@@ -49367,12 +49437,12 @@
       <c r="AB2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="AC2" s="105" t="s">
+      <c r="AC2" s="53" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="106">
+      <c r="A3" s="54">
         <v>2010</v>
       </c>
       <c r="B3" s="4">
@@ -49427,7 +49497,7 @@
         <f>発電電力量!N3/eELE!N$12</f>
         <v>1.2948860195235742E-2</v>
       </c>
-      <c r="O3" s="105">
+      <c r="O3" s="53">
         <f>SUM(B3:N3)</f>
         <v>18.520508905164583</v>
       </c>
@@ -49483,13 +49553,13 @@
         <f>発電電力量!AA3/eELE!N$12</f>
         <v>1.2948860195235742E-2</v>
       </c>
-      <c r="AC3" s="105">
+      <c r="AC3" s="53">
         <f>SUM(P3:AB3)</f>
         <v>18.520508905164583</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="107">
+      <c r="A4" s="55">
         <v>2020</v>
       </c>
       <c r="B4">
@@ -49606,7 +49676,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="107">
+      <c r="A5" s="55">
         <v>2030</v>
       </c>
       <c r="B5">
@@ -49723,7 +49793,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="107">
+      <c r="A6" s="55">
         <v>2040</v>
       </c>
       <c r="B6">
@@ -49840,7 +49910,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="108">
+      <c r="A7" s="56">
         <v>2050</v>
       </c>
       <c r="B7" s="5">
@@ -49984,40 +50054,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="109"/>
-      <c r="B1" s="173" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="174"/>
-      <c r="O1" s="173" t="s">
+      <c r="A1" s="57"/>
+      <c r="B1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="174"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="77"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="108"/>
+      <c r="A2" s="56"/>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
@@ -50054,7 +50124,7 @@
       <c r="M2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="N2" s="105" t="s">
+      <c r="N2" s="53" t="s">
         <v>84</v>
       </c>
       <c r="O2" s="4" t="s">
@@ -50093,12 +50163,12 @@
       <c r="Z2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="AA2" s="105" t="s">
+      <c r="AA2" s="53" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="107">
+      <c r="A3" s="55">
         <v>2010</v>
       </c>
       <c r="B3" s="4">
@@ -50149,7 +50219,7 @@
         <f>sELE!M3*最終エネルギー消費!$G23/LOSS!$B$12</f>
         <v>1.4677567751641748E-2</v>
       </c>
-      <c r="N3" s="105">
+      <c r="N3" s="53">
         <f>sELE!N3*最終エネルギー消費!$G23/LOSS!$B$12</f>
         <v>1.2948860195235742E-2</v>
       </c>
@@ -50201,13 +50271,13 @@
         <f>sELE!Z3*最終エネルギー消費!$L23/LOSS!$B$12</f>
         <v>1.4677567751641748E-2</v>
       </c>
-      <c r="AA3" s="105">
+      <c r="AA3" s="53">
         <f>sELE!AA3*最終エネルギー消費!$L23/LOSS!$B$12</f>
         <v>1.2948860195235742E-2</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="107">
+      <c r="A4" s="55">
         <v>2020</v>
       </c>
       <c r="B4">
@@ -50316,7 +50386,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="107">
+      <c r="A5" s="55">
         <v>2030</v>
       </c>
       <c r="B5">
@@ -50425,7 +50495,7 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="107">
+      <c r="A6" s="55">
         <v>2040</v>
       </c>
       <c r="B6">
@@ -50534,7 +50604,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="108">
+      <c r="A7" s="56">
         <v>2050</v>
       </c>
       <c r="B7" s="5">
@@ -50671,22 +50741,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="30">
         <v>2010</v>
       </c>
-      <c r="C1" s="31">
+      <c r="C1" s="30">
         <v>2020</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>93</v>
       </c>
     </row>
@@ -50694,46 +50764,46 @@
       <c r="A2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <f>[1]部門別CO2排出量!P3</f>
         <v>269.51474216725944</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="28">
         <f>[1]部門別CO2排出量!P4</f>
         <v>209.4235083709562</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="28">
         <v>257.81349782866999</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="28">
         <f>部門別CO2排出量!P7</f>
         <v>260.01618074402859</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="28">
         <f>部門別CO2排出量!AD7</f>
         <v>260.01618074402859</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <f>[1]部門別CO2排出量!P8</f>
         <v>249.02275586606845</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="32">
         <f>[1]部門別CO2排出量!P9</f>
         <v>196.15609230500672</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="32">
         <v>170.69003462550376</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="32">
         <f>部門別CO2排出量!P12</f>
         <v>210.67040851814829</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <f>部門別CO2排出量!AD12</f>
         <v>210.67040851814829</v>
       </c>
@@ -50742,46 +50812,46 @@
       <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="28">
         <f>[1]部門別CO2排出量!P13</f>
         <v>63.618347666356769</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="28">
         <f>[1]部門別CO2排出量!P14</f>
         <v>52.883709709806709</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <v>65.1157721973603</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="28">
         <f>部門別CO2排出量!P17</f>
         <v>66.032474177397248</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="28">
         <f>部門別CO2排出量!AD17</f>
         <v>66.032474177397248</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="32">
         <f>[1]部門別CO2排出量!P18</f>
         <v>69.588005432578569</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="32">
         <f>[1]部門別CO2排出量!P14</f>
         <v>52.883709709806709</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <v>52.398256859873904</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <f>部門別CO2排出量!P22</f>
         <v>52.527941152998537</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <f>部門別CO2排出量!AD22</f>
         <v>52.527941152998537</v>
       </c>
@@ -50790,46 +50860,46 @@
       <c r="A6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <f>部門別CO2排出量!P23</f>
         <v>476.37955455993358</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <f>部門別CO2排出量!P24</f>
         <v>449.00553720294573</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>502.31165964392062</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <f>部門別CO2排出量!P27</f>
         <v>496.52581315955877</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <f>部門別CO2排出量!AD27</f>
         <v>496.52581315955877</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <f>[1]部門別CO2排出量!P28</f>
         <v>28.775119328906975</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <f>[1]部門別CO2排出量!P29</f>
         <v>25.99212785621209</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <v>22.617687534623279</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <f>部門別CO2排出量!P32</f>
         <v>22.660005374260319</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <f>部門別CO2排出量!AD32</f>
         <v>22.660005374260319</v>
       </c>
@@ -50838,44 +50908,44 @@
       <c r="A8" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="28">
         <f>[1]部門別CO2排出量!P33</f>
         <v>29.46362437612942</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <f>[1]部門別CO2排出量!P34</f>
         <v>31.085649151718691</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>27.049940013143782</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <f>部門別CO2排出量!P37</f>
         <v>27.100550625829783</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="28">
         <f>部門別CO2排出量!AD37</f>
         <v>27.100550625829783</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>-46</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>-46</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>-46</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <f>部門別CO2排出量!P42</f>
         <v>-46</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <f>部門別CO2排出量!AD42</f>
         <v>-46</v>
       </c>
@@ -50884,23 +50954,23 @@
       <c r="A10" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="28">
         <f>SUM(B2:B9)</f>
         <v>1140.3621493972332</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="28">
         <f>SUM(C2:C9)</f>
         <v>971.43033430645278</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <f>SUM(D2:D9)</f>
         <v>1051.9968487030956</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="28">
         <f>SUM(E2:E9)</f>
         <v>1089.5333737522215</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="28">
         <f>SUM(F2:F9)</f>
         <v>1089.5333737522215</v>
       </c>
@@ -50930,71 +51000,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176" t="s">
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="175" t="s">
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="AC1" s="175"/>
-      <c r="AD1" s="175"/>
-      <c r="AE1" s="175"/>
-      <c r="AF1" s="175"/>
-      <c r="AG1" s="175" t="s">
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" s="175"/>
-      <c r="AI1" s="175"/>
-      <c r="AJ1" s="175"/>
-      <c r="AK1" s="175"/>
-      <c r="AL1" s="175" t="s">
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" s="175"/>
-      <c r="AN1" s="175"/>
-      <c r="AO1" s="175"/>
-      <c r="AP1" s="175"/>
-      <c r="AQ1" s="175" t="s">
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="AR1" s="175"/>
-      <c r="AS1" s="175"/>
-      <c r="AT1" s="175"/>
-      <c r="AU1" s="175"/>
-      <c r="AV1" s="175" t="s">
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="AW1" s="175"/>
-      <c r="AX1" s="175"/>
-      <c r="AY1" s="175"/>
-      <c r="AZ1" s="175"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
@@ -53009,71 +53079,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176" t="s">
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="175" t="s">
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="AC1" s="175"/>
-      <c r="AD1" s="175"/>
-      <c r="AE1" s="175"/>
-      <c r="AF1" s="175"/>
-      <c r="AG1" s="175" t="s">
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" s="175"/>
-      <c r="AI1" s="175"/>
-      <c r="AJ1" s="175"/>
-      <c r="AK1" s="175"/>
-      <c r="AL1" s="175" t="s">
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" s="175"/>
-      <c r="AN1" s="175"/>
-      <c r="AO1" s="175"/>
-      <c r="AP1" s="175"/>
-      <c r="AQ1" s="175" t="s">
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="AR1" s="175"/>
-      <c r="AS1" s="175"/>
-      <c r="AT1" s="175"/>
-      <c r="AU1" s="175"/>
-      <c r="AV1" s="175" t="s">
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="AW1" s="175"/>
-      <c r="AX1" s="175"/>
-      <c r="AY1" s="175"/>
-      <c r="AZ1" s="175"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
@@ -55094,38 +55164,38 @@
     <row r="1" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="177" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="177" t="s">
+      <c r="C1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="173"/>
-      <c r="AD1" s="174"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="77"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8"/>

</xml_diff>

<commit_message>
modify residential sector 2010 emission
</commit_message>
<xml_diff>
--- a/xlsx/model2.xlsx
+++ b/xlsx/model2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\TA\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FB9BFB-FA5E-47B7-A090-8212B690E68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7A29AF-6BAB-4DC6-8959-354C21DEC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2385" windowWidth="29040" windowHeight="15720" tabRatio="878" activeTab="5" xr2:uid="{BCC5EA96-140E-4D1F-AEAE-F8AA11DA45EB}"/>
+    <workbookView xWindow="38280" yWindow="2385" windowWidth="29040" windowHeight="15720" tabRatio="878" xr2:uid="{BCC5EA96-140E-4D1F-AEAE-F8AA11DA45EB}"/>
   </bookViews>
   <sheets>
     <sheet name="シナリオ" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="CO2排出量" sheetId="59" r:id="rId5"/>
     <sheet name="グラフ作成用" sheetId="58" r:id="rId6"/>
     <sheet name="スライド作成用" sheetId="64" state="hidden" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="62" state="hidden" r:id="rId8"/>
-    <sheet name="部門別CO2排出量" sheetId="12" state="hidden" r:id="rId9"/>
+    <sheet name="部門別CO2排出量" sheetId="12" state="hidden" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="62" state="hidden" r:id="rId9"/>
     <sheet name="GDP・POP" sheetId="30" state="hidden" r:id="rId10"/>
     <sheet name="COMFLOOR" sheetId="31" state="hidden" r:id="rId11"/>
     <sheet name="Intensity" sheetId="32" state="hidden" r:id="rId12"/>
@@ -1614,6 +1614,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1622,13 +1629,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10856,7 +10856,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1024.2639946178085</c:v>
+                  <c:v>1088.8477107592512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>942.06823852743798</c:v>
@@ -10937,7 +10937,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1024.2639946178085</c:v>
+                  <c:v>1088.8477107592512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>942.06823852743798</c:v>
@@ -11018,7 +11018,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1024.2639946178085</c:v>
+                  <c:v>1088.8477107592512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>942.06823852743798</c:v>
@@ -12776,7 +12776,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1024.2639946178085</c:v>
+                  <c:v>1088.8477107592512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>942.06823852743798</c:v>
@@ -12889,7 +12889,7 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>1024.2639946178085</c:v>
+                        <c:v>1088.8477107592512</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>942.06823852743798</c:v>
@@ -12990,7 +12990,7 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>1024.2639946178085</c:v>
+                        <c:v>1088.8477107592512</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>942.06823852743798</c:v>
@@ -14463,13 +14463,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>269.51474216725944</c:v>
+                  <c:v>261.62375155499154</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209.4235083709562</c:v>
+                  <c:v>203.84312748463603</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>260.01618074402859</c:v>
+                  <c:v>253.11561083538152</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>253.11561083538152</c:v>
@@ -14538,13 +14538,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>249.02275586606845</c:v>
+                  <c:v>222.98731447362985</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196.15609230500672</c:v>
+                  <c:v>175.63472635816763</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>171.17582078035531</c:v>
+                  <c:v>188.62350530113275</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>188.62350530113275</c:v>
@@ -14613,13 +14613,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>63.618347666356769</c:v>
+                  <c:v>59.181109031557583</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.883709709806709</c:v>
+                  <c:v>49.176064907319116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66.032474177397248</c:v>
+                  <c:v>61.373388455821313</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>61.373388455821313</c:v>
@@ -14688,13 +14688,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>69.588005432578569</c:v>
+                  <c:v>64.583716141442622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.883709709806709</c:v>
+                  <c:v>56.215623862257246</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.527941152998537</c:v>
+                  <c:v>49.012576322324165</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>49.012576322324165</c:v>
@@ -14766,13 +14766,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>476.37955455993358</c:v>
+                  <c:v>468.23307585259306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>449.00553720294573</c:v>
+                  <c:v>446.12091890712719</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>495.09542778752109</c:v>
+                  <c:v>493.52193172968884</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>493.52193172968884</c:v>
@@ -18713,7 +18713,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1024.2639946178085</c:v>
+                  <c:v>1088.8477107592512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>942.06823852743798</c:v>
@@ -18794,7 +18794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1024.2639946178085</c:v>
+                  <c:v>1088.8477107592512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>942.06823852743798</c:v>
@@ -18875,7 +18875,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1024.2639946178085</c:v>
+                  <c:v>1088.8477107592512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>942.06823852743798</c:v>
@@ -19304,10 +19304,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>269.51474216725944</c:v>
+                  <c:v>261.62375155499154</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209.4235083709562</c:v>
+                  <c:v>203.84312748463603</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>253.11561083538152</c:v>
@@ -19380,10 +19380,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>249.02275586606845</c:v>
+                  <c:v>222.98731447362985</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196.15609230500672</c:v>
+                  <c:v>175.63472635816763</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>188.62350530113275</c:v>
@@ -19456,10 +19456,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>63.618347666356769</c:v>
+                  <c:v>59.181109031557583</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.883709709806709</c:v>
+                  <c:v>49.176064907319116</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>61.373388455821313</c:v>
@@ -19532,10 +19532,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>69.588005432578569</c:v>
+                  <c:v>64.583716141442622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.883709709806709</c:v>
+                  <c:v>56.215623862257246</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>49.012576322324165</c:v>
@@ -19611,10 +19611,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>476.37955455993358</c:v>
+                  <c:v>468.23307585259306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>449.00553720294573</c:v>
+                  <c:v>446.12091890712719</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>493.52193172968884</c:v>
@@ -24827,10 +24827,10 @@
   </sheetPr>
   <dimension ref="A1:AG80"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -25008,11 +25008,11 @@
       </c>
       <c r="AC6" s="36">
         <f>CO2排出量!B2</f>
-        <v>269.51474216725944</v>
+        <v>261.62375155499154</v>
       </c>
       <c r="AD6" s="42">
         <f>CO2排出量!C2</f>
-        <v>209.4235083709562</v>
+        <v>203.84312748463603</v>
       </c>
       <c r="AE6" s="36">
         <v>253.11561083538152</v>
@@ -25051,11 +25051,11 @@
       </c>
       <c r="AC7" s="35">
         <f>CO2排出量!B3</f>
-        <v>249.02275586606845</v>
+        <v>222.98731447362985</v>
       </c>
       <c r="AD7" s="43">
         <f>CO2排出量!C3</f>
-        <v>196.15609230500672</v>
+        <v>175.63472635816763</v>
       </c>
       <c r="AE7" s="35">
         <v>188.62350530113275</v>
@@ -25094,11 +25094,11 @@
       </c>
       <c r="AC8" s="34">
         <f>CO2排出量!B4</f>
-        <v>63.618347666356769</v>
+        <v>59.181109031557583</v>
       </c>
       <c r="AD8" s="44">
         <f>CO2排出量!C4</f>
-        <v>52.883709709806709</v>
+        <v>49.176064907319116</v>
       </c>
       <c r="AE8" s="34">
         <v>61.373388455821313</v>
@@ -25148,11 +25148,11 @@
       </c>
       <c r="AC9" s="35">
         <f>CO2排出量!B5</f>
-        <v>69.588005432578569</v>
+        <v>64.583716141442622</v>
       </c>
       <c r="AD9" s="43">
         <f>CO2排出量!C5</f>
-        <v>52.883709709806709</v>
+        <v>56.215623862257246</v>
       </c>
       <c r="AE9" s="35">
         <v>49.012576322324165</v>
@@ -25192,11 +25192,11 @@
       </c>
       <c r="AC10" s="34">
         <f>CO2排出量!B6</f>
-        <v>476.37955455993358</v>
+        <v>468.23307585259306</v>
       </c>
       <c r="AD10" s="44">
         <f>CO2排出量!C6</f>
-        <v>449.00553720294573</v>
+        <v>446.12091890712719</v>
       </c>
       <c r="AE10" s="34">
         <v>493.52193172968884</v>
@@ -25376,11 +25376,11 @@
       </c>
       <c r="AC14" s="40">
         <f>CO2排出量!B10</f>
-        <v>1140.3621493972332</v>
+        <v>1088.8477107592512</v>
       </c>
       <c r="AD14" s="45">
         <f>CO2排出量!C10</f>
-        <v>971.43033430645278</v>
+        <v>942.06823852743798</v>
       </c>
       <c r="AE14" s="40">
         <v>1049.4075686444387</v>
@@ -26240,15 +26240,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6:AG14">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AG5">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43499,7 +43499,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -50920,7 +50920,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -50954,10 +50954,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="28">
-        <v>269.51474216725944</v>
+        <f>部門別CO2排出量!P3</f>
+        <v>261.62375155499154</v>
       </c>
       <c r="C2" s="28">
-        <v>209.4235083709562</v>
+        <f>部門別CO2排出量!P4</f>
+        <v>203.84312748463603</v>
       </c>
       <c r="D2" s="28">
         <v>253.11561083538152</v>
@@ -50976,10 +50978,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="32">
-        <v>249.02275586606845</v>
+        <f>部門別CO2排出量!P8</f>
+        <v>222.98731447362985</v>
       </c>
       <c r="C3" s="32">
-        <v>196.15609230500672</v>
+        <f>部門別CO2排出量!P9</f>
+        <v>175.63472635816763</v>
       </c>
       <c r="D3" s="32">
         <v>188.62350530113275</v>
@@ -50998,10 +51002,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="28">
-        <v>63.618347666356769</v>
+        <f>部門別CO2排出量!P13</f>
+        <v>59.181109031557583</v>
       </c>
       <c r="C4" s="28">
-        <v>52.883709709806709</v>
+        <f>部門別CO2排出量!P14</f>
+        <v>49.176064907319116</v>
       </c>
       <c r="D4" s="28">
         <v>61.373388455821313</v>
@@ -51020,10 +51026,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="32">
-        <v>69.588005432578569</v>
+        <f>部門別CO2排出量!P18</f>
+        <v>64.583716141442622</v>
       </c>
       <c r="C5" s="32">
-        <v>52.883709709806709</v>
+        <f>部門別CO2排出量!P19</f>
+        <v>56.215623862257246</v>
       </c>
       <c r="D5" s="32">
         <v>49.012576322324165</v>
@@ -51042,10 +51050,12 @@
         <v>30</v>
       </c>
       <c r="B6" s="28">
-        <v>476.37955455993358</v>
+        <f>部門別CO2排出量!P23</f>
+        <v>468.23307585259306</v>
       </c>
       <c r="C6" s="28">
-        <v>449.00553720294573</v>
+        <f>部門別CO2排出量!P24</f>
+        <v>446.12091890712719</v>
       </c>
       <c r="D6" s="28">
         <v>493.52193172968884</v>
@@ -51130,10 +51140,12 @@
         <v>27</v>
       </c>
       <c r="B10" s="28">
-        <v>1140.3621493972332</v>
+        <f>SUM(B2:B9)</f>
+        <v>1088.8477107592512</v>
       </c>
       <c r="C10" s="28">
-        <v>971.43033430645278</v>
+        <f>SUM(C2:C9)</f>
+        <v>942.06823852743798</v>
       </c>
       <c r="D10" s="28">
         <v>1049.4075686444387</v>
@@ -51161,8 +51173,8 @@
   </sheetPr>
   <dimension ref="A1:AZ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -52442,26 +52454,26 @@
         <v>2010</v>
       </c>
       <c r="B11" s="2">
-        <v>1024.2639946178085</v>
+        <v>1088.8477107592512</v>
       </c>
       <c r="C11" s="2">
         <f>部門別CO2排出量!P43</f>
-        <v>1024.2639946178085</v>
+        <v>1088.8477107592512</v>
       </c>
       <c r="D11" s="2">
         <f>部門別CO2排出量!AD43</f>
-        <v>1024.2639946178085</v>
+        <v>1088.8477107592512</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G11">
         <f>CO2排出量!B2</f>
-        <v>269.51474216725944</v>
+        <v>261.62375155499154</v>
       </c>
       <c r="H11">
         <f>CO2排出量!C2</f>
-        <v>209.4235083709562</v>
+        <v>203.84312748463603</v>
       </c>
       <c r="I11">
         <v>253.11561083538152</v>
@@ -52495,11 +52507,11 @@
       </c>
       <c r="G12">
         <f>CO2排出量!B3</f>
-        <v>249.02275586606845</v>
+        <v>222.98731447362985</v>
       </c>
       <c r="H12">
         <f>CO2排出量!C3</f>
-        <v>196.15609230500672</v>
+        <v>175.63472635816763</v>
       </c>
       <c r="I12">
         <v>188.62350530113275</v>
@@ -52533,11 +52545,11 @@
       </c>
       <c r="G13">
         <f>CO2排出量!B4</f>
-        <v>63.618347666356769</v>
+        <v>59.181109031557583</v>
       </c>
       <c r="H13">
         <f>CO2排出量!C4</f>
-        <v>52.883709709806709</v>
+        <v>49.176064907319116</v>
       </c>
       <c r="I13">
         <v>61.373388455821313</v>
@@ -52571,11 +52583,11 @@
       </c>
       <c r="G14">
         <f>CO2排出量!B5</f>
-        <v>69.588005432578569</v>
+        <v>64.583716141442622</v>
       </c>
       <c r="H14">
         <f>CO2排出量!C5</f>
-        <v>52.883709709806709</v>
+        <v>56.215623862257246</v>
       </c>
       <c r="I14">
         <v>49.012576322324165</v>
@@ -52609,11 +52621,11 @@
       </c>
       <c r="G15">
         <f>CO2排出量!B6</f>
-        <v>476.37955455993358</v>
+        <v>468.23307585259306</v>
       </c>
       <c r="H15">
         <f>CO2排出量!C6</f>
-        <v>449.00553720294573</v>
+        <v>446.12091890712719</v>
       </c>
       <c r="I15">
         <v>493.52193172968884</v>
@@ -53240,8 +53252,8 @@
   </sheetPr>
   <dimension ref="A1:AZ61"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -54517,29 +54529,30 @@
         <v>2010</v>
       </c>
       <c r="B11" s="2">
-        <v>1070.7741439646547</v>
+        <v>1024.2639946178085</v>
       </c>
       <c r="C11" s="2">
         <f>部門別CO2排出量!P43</f>
-        <v>1024.2639946178085</v>
+        <v>1088.8477107592512</v>
       </c>
       <c r="D11" s="2">
         <f>部門別CO2排出量!AD43</f>
-        <v>1024.2639946178085</v>
+        <v>1088.8477107592512</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G11">
         <f>CO2排出量!B2</f>
-        <v>269.51474216725944</v>
+        <v>261.62375155499154</v>
       </c>
       <c r="H11">
         <f>CO2排出量!C2</f>
-        <v>209.4235083709562</v>
+        <v>203.84312748463603</v>
       </c>
       <c r="I11">
-        <v>260.01618074402859</v>
+        <f>CO2排出量!D2</f>
+        <v>253.11561083538152</v>
       </c>
       <c r="J11">
         <f>CO2排出量!E2</f>
@@ -54555,7 +54568,7 @@
         <v>2020</v>
       </c>
       <c r="B12" s="2">
-        <v>978.76242648442167</v>
+        <v>942.06823852743798</v>
       </c>
       <c r="C12" s="2">
         <f>部門別CO2排出量!P44</f>
@@ -54570,14 +54583,15 @@
       </c>
       <c r="G12">
         <f>CO2排出量!B3</f>
-        <v>249.02275586606845</v>
+        <v>222.98731447362985</v>
       </c>
       <c r="H12">
         <f>CO2排出量!C3</f>
-        <v>196.15609230500672</v>
+        <v>175.63472635816763</v>
       </c>
       <c r="I12">
-        <v>171.17582078035531</v>
+        <f>CO2排出量!D3</f>
+        <v>188.62350530113275</v>
       </c>
       <c r="J12">
         <f>CO2排出量!E3</f>
@@ -54593,7 +54607,7 @@
         <v>2030</v>
       </c>
       <c r="B13" s="2">
-        <v>1007.4537582833925</v>
+        <v>984.39591573841176</v>
       </c>
       <c r="C13" s="2">
         <f>部門別CO2排出量!P45</f>
@@ -54608,14 +54622,15 @@
       </c>
       <c r="G13">
         <f>CO2排出量!B4</f>
-        <v>63.618347666356769</v>
+        <v>59.181109031557583</v>
       </c>
       <c r="H13">
         <f>CO2排出量!C4</f>
-        <v>52.883709709806709</v>
+        <v>49.176064907319116</v>
       </c>
       <c r="I13">
-        <v>66.032474177397248</v>
+        <f>CO2排出量!D4</f>
+        <v>61.373388455821313</v>
       </c>
       <c r="J13">
         <f>CO2排出量!E4</f>
@@ -54631,7 +54646,7 @@
         <v>2040</v>
       </c>
       <c r="B14" s="2">
-        <v>1026.3482276252621</v>
+        <v>1015.8856723562906</v>
       </c>
       <c r="C14" s="2">
         <f>部門別CO2排出量!P46</f>
@@ -54646,14 +54661,15 @@
       </c>
       <c r="G14">
         <f>CO2排出量!B5</f>
-        <v>69.588005432578569</v>
+        <v>64.583716141442622</v>
       </c>
       <c r="H14">
         <f>CO2排出量!C5</f>
-        <v>52.883709709806709</v>
+        <v>56.215623862257246</v>
       </c>
       <c r="I14">
-        <v>52.527941152998537</v>
+        <f>CO2排出量!D5</f>
+        <v>49.012576322324165</v>
       </c>
       <c r="J14">
         <f>CO2排出量!E5</f>
@@ -54669,7 +54685,7 @@
         <v>2050</v>
       </c>
       <c r="B15" s="2">
-        <v>1048.6084006423907</v>
+        <v>1049.4075686444387</v>
       </c>
       <c r="C15" s="2">
         <f>部門別CO2排出量!P47</f>
@@ -54684,14 +54700,15 @@
       </c>
       <c r="G15">
         <f>CO2排出量!B6</f>
-        <v>476.37955455993358</v>
+        <v>468.23307585259306</v>
       </c>
       <c r="H15">
         <f>CO2排出量!C6</f>
-        <v>449.00553720294573</v>
+        <v>446.12091890712719</v>
       </c>
       <c r="I15">
-        <v>495.09542778752109</v>
+        <f>CO2排出量!D6</f>
+        <v>493.52193172968884</v>
       </c>
       <c r="J15">
         <f>CO2排出量!E6</f>
@@ -54719,6 +54736,7 @@
         <v>25.99212785621209</v>
       </c>
       <c r="I16">
+        <f>CO2排出量!D7</f>
         <v>22.660005374260319</v>
       </c>
       <c r="J16">
@@ -54757,6 +54775,7 @@
         <v>31.085649151718691</v>
       </c>
       <c r="I17">
+        <f>CO2排出量!D8</f>
         <v>27.100550625829783</v>
       </c>
       <c r="J17">
@@ -54795,6 +54814,7 @@
         <v>-46</v>
       </c>
       <c r="I18">
+        <f>CO2排出量!D9</f>
         <v>-46</v>
       </c>
       <c r="J18">
@@ -55308,27 +55328,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899B19A5-7503-4513-BF71-2D7E23416D9A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O104" sqref="O104"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACBDC0A-B774-4127-9811-6E05EDCA9F07}">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -56040,10 +56044,38 @@
       <c r="B18">
         <v>2010</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="9"/>
-      <c r="AD18" s="3"/>
+      <c r="C18" s="9">
+        <f>最終エネルギー消費!C18*EMF!$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>最終エネルギー消費!D18*EMF!$C$2</f>
+        <v>42.814475046385361</v>
+      </c>
+      <c r="G18">
+        <f>最終エネルギー消費!E18*EMF!$E$2</f>
+        <v>21.769241095057257</v>
+      </c>
+      <c r="P18" s="3">
+        <f t="shared" si="2"/>
+        <v>64.583716141442622</v>
+      </c>
+      <c r="Q18" s="9">
+        <f>最終エネルギー消費!H18*EMF!$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f>最終エネルギー消費!I18*EMF!$C$2</f>
+        <v>42.814475046385361</v>
+      </c>
+      <c r="U18">
+        <f>最終エネルギー消費!J18*EMF!$E$2</f>
+        <v>21.769241095057257</v>
+      </c>
+      <c r="AD18" s="3">
+        <f t="shared" si="3"/>
+        <v>64.583716141442622</v>
+      </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A19" s="9"/>
@@ -57052,7 +57084,7 @@
       </c>
       <c r="E43">
         <f t="shared" si="10"/>
-        <v>397.92016663412517</v>
+        <v>440.73464168051055</v>
       </c>
       <c r="F43">
         <f t="shared" si="10"/>
@@ -57060,7 +57092,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="10"/>
-        <v>176.91658111172131</v>
+        <v>198.6858222067786</v>
       </c>
       <c r="H43">
         <f t="shared" si="10"/>
@@ -57075,7 +57107,7 @@
         <v>0</v>
       </c>
       <c r="K43">
-        <f t="shared" si="10"/>
+        <f>SUM(K3,K8,K13,K18,K23,K28,K33,K38)</f>
         <v>0</v>
       </c>
       <c r="L43">
@@ -57096,10 +57128,10 @@
       </c>
       <c r="P43" s="3">
         <f t="shared" si="10"/>
-        <v>1024.2639946178085</v>
+        <v>1088.8477107592512</v>
       </c>
       <c r="Q43" s="9">
-        <f t="shared" si="10"/>
+        <f>SUM(Q3,Q8,Q13,Q18,Q23,Q28,Q33,Q38)</f>
         <v>437.18850316692556</v>
       </c>
       <c r="R43">
@@ -57108,7 +57140,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="10"/>
-        <v>397.92016663412517</v>
+        <v>440.73464168051055</v>
       </c>
       <c r="T43">
         <f t="shared" si="10"/>
@@ -57116,7 +57148,7 @@
       </c>
       <c r="U43">
         <f t="shared" si="10"/>
-        <v>176.91658111172131</v>
+        <v>198.6858222067786</v>
       </c>
       <c r="V43">
         <f t="shared" si="10"/>
@@ -57152,7 +57184,7 @@
       </c>
       <c r="AD43" s="3">
         <f>SUM(AD3,AD8,AD13,AD18,AD23,AD28,AD33,AD38)</f>
-        <v>1024.2639946178085</v>
+        <v>1088.8477107592512</v>
       </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.4">
@@ -57217,7 +57249,7 @@
         <v>942.06823852743798</v>
       </c>
       <c r="Q44" s="9">
-        <f t="shared" si="11"/>
+        <f>SUM(Q4,Q9,Q14,Q19,Q24,Q29,Q34,Q39)</f>
         <v>397.28773460765638</v>
       </c>
       <c r="R44">
@@ -57635,4 +57667,20 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899B19A5-7503-4513-BF71-2D7E23416D9A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K99" sqref="K99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>